<commit_message>
update meta data and symbols
</commit_message>
<xml_diff>
--- a/NOAKADEXPI_TestPlan.xlsx
+++ b/NOAKADEXPI_TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dragaas-my.sharepoint.com/personal/tonia_pedersen_draga_no/Documents/Documents/GitHub/DEXPI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DEXPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="435" documentId="8_{42884457-2C83-42E6-ACC8-ECDCE8C39558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F3FD9F6-21F3-429A-8F76-629B3E7CB27B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772833EC-F3F2-4C2E-A0E0-A288851FD639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="287">
   <si>
     <t>Considerations:</t>
   </si>
@@ -292,9 +292,6 @@
     <t>DrawingName</t>
   </si>
   <si>
-    <t>FileName</t>
-  </si>
-  <si>
     <t>ProcessPlantIdentificationCode</t>
   </si>
   <si>
@@ -881,6 +878,33 @@
   </si>
   <si>
     <t>Check error log from Verificator</t>
+  </si>
+  <si>
+    <t>**Not required as this is covered by the Verificator</t>
+  </si>
+  <si>
+    <t>DrawingSubTitle</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>PIPING AND INSTRUMENT DIAGRAM</t>
+  </si>
+  <si>
+    <t>TEST P&amp;ID</t>
+  </si>
+  <si>
+    <t>KRAFLA</t>
+  </si>
+  <si>
+    <t>20.10.21</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>NTS at A1</t>
   </si>
 </sst>
 </file>
@@ -1471,7 +1495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1810,6 +1834,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1981,6 +2024,68 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28729</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>97923</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4104970" cy="937629"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EFA884E-8EAB-4EC1-BB98-7FC088B906F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19986733">
+          <a:off x="885979" y="2336298"/>
+          <a:ext cx="4104970" cy="937629"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="5400" b="1" cap="none" spc="50">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:innerShdw blurRad="63500" dist="50800" dir="13500000">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:innerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Not Required</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2251,12 +2356,12 @@
   </sheetPr>
   <dimension ref="B1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,7 +2428,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -2351,7 +2456,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="145" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -2519,7 +2624,7 @@
         <v>56</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D24" s="126" t="s">
         <v>57</v>
@@ -2535,7 +2640,7 @@
         <v>58</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D25" s="126" t="s">
         <v>60</v>
@@ -2551,7 +2656,7 @@
         <v>61</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26" s="126" t="s">
         <v>62</v>
@@ -2563,13 +2668,13 @@
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="95" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D27" s="126" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E27" s="41"/>
       <c r="F27" s="7"/>
@@ -2578,13 +2683,13 @@
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="95" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D28" s="127" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E28" s="41"/>
       <c r="F28" s="71"/>
@@ -2594,13 +2699,13 @@
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="95" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D29" s="127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E29" s="41"/>
       <c r="F29" s="71"/>
@@ -2637,7 +2742,7 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="93" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C33" s="32" t="s">
         <v>27</v>
@@ -2651,13 +2756,13 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="95" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D34" s="127" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E34" s="41"/>
       <c r="F34" s="71"/>
@@ -2666,13 +2771,13 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="95" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D35" s="127" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E35" s="41"/>
       <c r="F35" s="71"/>
@@ -2682,13 +2787,13 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="95" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" s="127" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E36" s="41"/>
       <c r="F36" s="71"/>
@@ -2697,13 +2802,13 @@
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="95" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D37" s="127" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E37" s="41"/>
       <c r="F37" s="71"/>
@@ -2712,13 +2817,13 @@
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="95" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D38" s="127" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E38" s="41"/>
       <c r="F38" s="71"/>
@@ -3152,7 +3257,7 @@
       </c>
       <c r="C4" s="153"/>
       <c r="D4" s="154" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E4" s="154"/>
       <c r="F4" s="154"/>
@@ -3165,7 +3270,7 @@
       </c>
       <c r="C5" s="158"/>
       <c r="D5" s="159" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" s="159"/>
       <c r="F5" s="159"/>
@@ -3214,7 +3319,7 @@
         <v>31</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H11" s="77" t="s">
         <v>23</v>
@@ -3452,7 +3557,7 @@
   <dimension ref="A2:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A11:XFD31"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -3543,7 +3648,7 @@
         <v>31</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H11" s="77" t="s">
         <v>23</v>
@@ -3788,7 +3893,7 @@
   <dimension ref="A2:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D6" sqref="D6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -3840,7 +3945,9 @@
         <v>19</v>
       </c>
       <c r="C6" s="158"/>
-      <c r="D6" s="159"/>
+      <c r="D6" s="159" t="s">
+        <v>278</v>
+      </c>
       <c r="E6" s="159"/>
       <c r="F6" s="159"/>
       <c r="G6" s="160"/>
@@ -3877,7 +3984,7 @@
         <v>31</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H11" s="77" t="s">
         <v>23</v>
@@ -3888,7 +3995,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15">
@@ -3902,7 +4009,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="81" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -3914,7 +4021,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="81" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -3926,7 +4033,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -3938,7 +4045,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -3950,7 +4057,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="81" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -3962,7 +4069,7 @@
         <v>7</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -3974,7 +4081,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="81" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -3986,7 +4093,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -3998,7 +4105,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="81" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -4010,7 +4117,7 @@
         <v>11</v>
       </c>
       <c r="D22" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -4022,7 +4129,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="81" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -4034,7 +4141,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E24" s="71"/>
       <c r="F24" s="7"/>
@@ -4046,7 +4153,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="81" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E25" s="71"/>
       <c r="F25" s="7"/>
@@ -4058,7 +4165,7 @@
         <v>15</v>
       </c>
       <c r="D26" s="81" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E26" s="71"/>
       <c r="F26" s="7"/>
@@ -4070,7 +4177,7 @@
         <v>16</v>
       </c>
       <c r="D27" s="81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E27" s="71"/>
       <c r="F27" s="7"/>
@@ -4082,7 +4189,7 @@
         <v>17</v>
       </c>
       <c r="D28" s="81" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E28" s="71"/>
       <c r="F28" s="7"/>
@@ -4094,7 +4201,7 @@
         <v>18</v>
       </c>
       <c r="D29" s="81" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E29" s="71"/>
       <c r="F29" s="7"/>
@@ -4106,7 +4213,7 @@
         <v>19</v>
       </c>
       <c r="D30" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E30" s="73"/>
       <c r="F30" s="23"/>
@@ -4139,6 +4246,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4146,8 +4254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124920C8-F026-4FD1-ADA0-B7CB0E8079B3}">
   <dimension ref="A2:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -4156,7 +4264,7 @@
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="47.140625" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="6" width="39.140625" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="162" customWidth="1"/>
     <col min="7" max="7" width="25.140625" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" customWidth="1"/>
@@ -4232,11 +4340,11 @@
       <c r="E11" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="76" t="s">
+      <c r="F11" s="163" t="s">
         <v>31</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H11" s="77" t="s">
         <v>23</v>
@@ -4250,7 +4358,9 @@
         <v>81</v>
       </c>
       <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="F12" s="164" t="s">
+        <v>281</v>
+      </c>
       <c r="G12" s="84"/>
       <c r="H12" s="25"/>
     </row>
@@ -4258,11 +4368,12 @@
       <c r="C13" s="20">
         <v>2</v>
       </c>
-      <c r="D13" s="81" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="D13" t="s">
+        <v>279</v>
+      </c>
+      <c r="F13" s="162" t="s">
+        <v>282</v>
+      </c>
       <c r="G13" s="14"/>
       <c r="H13" s="19"/>
     </row>
@@ -4271,10 +4382,12 @@
         <v>3</v>
       </c>
       <c r="D14" s="81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="165" t="s">
+        <v>280</v>
+      </c>
       <c r="G14" s="14"/>
       <c r="H14" s="19"/>
     </row>
@@ -4283,10 +4396,12 @@
         <v>4</v>
       </c>
       <c r="D15" s="81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="F15" s="165" t="s">
+        <v>283</v>
+      </c>
       <c r="G15" s="14"/>
       <c r="H15" s="19"/>
     </row>
@@ -4295,10 +4410,12 @@
         <v>5</v>
       </c>
       <c r="D16" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="165">
+        <v>20</v>
+      </c>
       <c r="G16" s="14"/>
       <c r="H16" s="19"/>
     </row>
@@ -4307,10 +4424,10 @@
         <v>6</v>
       </c>
       <c r="D17" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="165"/>
       <c r="G17" s="14"/>
       <c r="H17" s="19"/>
     </row>
@@ -4319,10 +4436,10 @@
         <v>7</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="F18" s="165"/>
       <c r="G18" s="14"/>
       <c r="H18" s="19"/>
     </row>
@@ -4331,10 +4448,10 @@
         <v>8</v>
       </c>
       <c r="D19" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="F19" s="165"/>
       <c r="G19" s="14"/>
       <c r="H19" s="19"/>
     </row>
@@ -4343,10 +4460,12 @@
         <v>9</v>
       </c>
       <c r="D20" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="F20" s="165" t="s">
+        <v>284</v>
+      </c>
       <c r="G20" s="14"/>
       <c r="H20" s="19"/>
     </row>
@@ -4355,10 +4474,12 @@
         <v>10</v>
       </c>
       <c r="D21" s="81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="F21" s="165" t="s">
+        <v>285</v>
+      </c>
       <c r="G21" s="14"/>
       <c r="H21" s="19"/>
     </row>
@@ -4367,10 +4488,12 @@
         <v>11</v>
       </c>
       <c r="D22" s="81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="165" t="s">
+        <v>286</v>
+      </c>
       <c r="G22" s="14"/>
       <c r="H22" s="19"/>
     </row>
@@ -4378,9 +4501,9 @@
       <c r="C23" s="20">
         <v>12</v>
       </c>
-      <c r="D23" s="81"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="D23" s="168" t="s">
+        <v>86</v>
+      </c>
       <c r="G23" s="14"/>
       <c r="H23" s="19"/>
     </row>
@@ -4388,9 +4511,9 @@
       <c r="C24" s="20">
         <v>13</v>
       </c>
-      <c r="D24" s="81"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="D24" s="168" t="s">
+        <v>87</v>
+      </c>
       <c r="G24" s="14"/>
       <c r="H24" s="19"/>
     </row>
@@ -4400,7 +4523,7 @@
       </c>
       <c r="D25" s="81"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="165"/>
       <c r="G25" s="14"/>
       <c r="H25" s="19"/>
     </row>
@@ -4410,7 +4533,7 @@
       </c>
       <c r="D26" s="81"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="165"/>
       <c r="G26" s="14"/>
       <c r="H26" s="19"/>
     </row>
@@ -4420,7 +4543,7 @@
       </c>
       <c r="D27" s="81"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="F27" s="165"/>
       <c r="G27" s="14"/>
       <c r="H27" s="19"/>
     </row>
@@ -4430,7 +4553,7 @@
       </c>
       <c r="D28" s="81"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="F28" s="165"/>
       <c r="G28" s="14"/>
       <c r="H28" s="19"/>
     </row>
@@ -4440,7 +4563,7 @@
       </c>
       <c r="D29" s="81"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="F29" s="165"/>
       <c r="G29" s="14"/>
       <c r="H29" s="19"/>
     </row>
@@ -4450,7 +4573,7 @@
       </c>
       <c r="D30" s="78"/>
       <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
+      <c r="F30" s="166"/>
       <c r="G30" s="85"/>
       <c r="H30" s="24"/>
     </row>
@@ -4461,7 +4584,7 @@
       <c r="C32" s="68"/>
       <c r="D32" s="68"/>
       <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
+      <c r="F32" s="167"/>
       <c r="G32" s="68"/>
       <c r="H32" s="68"/>
       <c r="I32" s="68"/>
@@ -4576,7 +4699,7 @@
         <v>31</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H11" s="77" t="s">
         <v>23</v>
@@ -4910,7 +5033,7 @@
         <v>31</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H11" s="77" t="s">
         <v>23</v>
@@ -4999,7 +5122,7 @@
         <v>7</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="71"/>
@@ -5011,7 +5134,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="81" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="71"/>
@@ -5023,7 +5146,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="81" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="71"/>
@@ -5035,7 +5158,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="81" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="71"/>
@@ -5047,7 +5170,7 @@
         <v>11</v>
       </c>
       <c r="D22" s="81" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="71"/>
@@ -5059,7 +5182,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="81" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="71"/>
@@ -5071,7 +5194,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="81" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -5083,7 +5206,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="81" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -5145,7 +5268,7 @@
       <c r="A32" s="151"/>
       <c r="B32" s="151"/>
       <c r="C32" s="140" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D32" s="68"/>
       <c r="E32" s="68"/>
@@ -5156,19 +5279,19 @@
     </row>
     <row r="33" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="83" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="83" t="s">
         <v>150</v>
       </c>
-      <c r="D33" s="83" t="s">
+      <c r="E33" s="83" t="s">
         <v>151</v>
       </c>
-      <c r="E33" s="83" t="s">
+      <c r="F33" s="83" t="s">
         <v>152</v>
       </c>
-      <c r="F33" s="83" t="s">
-        <v>153</v>
-      </c>
       <c r="G33" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H33" s="77" t="s">
         <v>23</v>
@@ -5176,80 +5299,80 @@
     </row>
     <row r="34" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C34" s="84" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" s="84" t="s">
         <v>154</v>
       </c>
-      <c r="D34" s="84" t="s">
+      <c r="E34" s="84" t="s">
         <v>155</v>
       </c>
-      <c r="E34" s="84" t="s">
+      <c r="F34" s="84" t="s">
         <v>156</v>
-      </c>
-      <c r="F34" s="84" t="s">
-        <v>157</v>
       </c>
       <c r="G34" s="84"/>
       <c r="H34" s="25"/>
     </row>
     <row r="35" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C35" s="84" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="84" t="s">
         <v>158</v>
       </c>
-      <c r="D35" s="84" t="s">
+      <c r="E35" s="84" t="s">
+        <v>155</v>
+      </c>
+      <c r="F35" s="84" t="s">
         <v>159</v>
-      </c>
-      <c r="E35" s="84" t="s">
-        <v>156</v>
-      </c>
-      <c r="F35" s="84" t="s">
-        <v>160</v>
       </c>
       <c r="G35" s="82"/>
       <c r="H35" s="72"/>
     </row>
     <row r="36" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C36" s="84" t="s">
+        <v>160</v>
+      </c>
+      <c r="D36" s="84" t="s">
         <v>161</v>
       </c>
-      <c r="D36" s="84" t="s">
+      <c r="E36" s="84" t="s">
         <v>162</v>
       </c>
-      <c r="E36" s="84" t="s">
+      <c r="F36" s="84" t="s">
         <v>163</v>
-      </c>
-      <c r="F36" s="84" t="s">
-        <v>164</v>
       </c>
       <c r="G36" s="82"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C37" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="D37" s="84" t="s">
         <v>165</v>
       </c>
-      <c r="D37" s="84" t="s">
+      <c r="E37" s="84" t="s">
         <v>166</v>
       </c>
-      <c r="E37" s="84" t="s">
+      <c r="F37" s="84" t="s">
         <v>167</v>
-      </c>
-      <c r="F37" s="84" t="s">
-        <v>168</v>
       </c>
       <c r="G37" s="82"/>
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C38" s="84" t="s">
+        <v>168</v>
+      </c>
+      <c r="D38" s="84" t="s">
         <v>169</v>
-      </c>
-      <c r="D38" s="84" t="s">
-        <v>170</v>
       </c>
       <c r="E38" s="84">
         <v>1</v>
       </c>
       <c r="F38" s="84" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G38" s="82"/>
       <c r="H38" s="72"/>
@@ -5274,7 +5397,7 @@
       <c r="A41" s="151"/>
       <c r="B41" s="151"/>
       <c r="C41" s="140" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D41" s="69"/>
       <c r="E41" s="69"/>
@@ -5285,19 +5408,19 @@
     </row>
     <row r="42" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="83" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D42" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="E42" s="83" t="s">
+        <v>150</v>
+      </c>
+      <c r="F42" s="83" t="s">
         <v>173</v>
       </c>
-      <c r="E42" s="83" t="s">
-        <v>151</v>
-      </c>
-      <c r="F42" s="83" t="s">
-        <v>174</v>
-      </c>
       <c r="G42" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H42" s="77" t="s">
         <v>23</v>
@@ -5305,96 +5428,96 @@
     </row>
     <row r="43" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="84" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D43" s="84" t="s">
+        <v>126</v>
+      </c>
+      <c r="E43" s="84" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="84" t="s">
+      <c r="F43" s="142" t="s">
         <v>128</v>
-      </c>
-      <c r="F43" s="142" t="s">
-        <v>129</v>
       </c>
       <c r="G43" s="84"/>
       <c r="H43" s="25"/>
     </row>
     <row r="44" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="84" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D44" s="84" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="84" t="s">
+        <v>127</v>
+      </c>
+      <c r="F44" s="143" t="s">
         <v>130</v>
-      </c>
-      <c r="E44" s="84" t="s">
-        <v>128</v>
-      </c>
-      <c r="F44" s="143" t="s">
-        <v>131</v>
       </c>
       <c r="G44" s="82"/>
       <c r="H44" s="72"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="84" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D45" s="84" t="s">
+        <v>131</v>
+      </c>
+      <c r="E45" s="84" t="s">
         <v>132</v>
       </c>
-      <c r="E45" s="84" t="s">
+      <c r="F45" s="143" t="s">
         <v>133</v>
-      </c>
-      <c r="F45" s="143" t="s">
-        <v>134</v>
       </c>
       <c r="G45" s="82"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="84" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D46" s="84" t="s">
+        <v>134</v>
+      </c>
+      <c r="E46" s="84" t="s">
         <v>135</v>
       </c>
-      <c r="E46" s="84" t="s">
+      <c r="F46" s="143" t="s">
         <v>136</v>
-      </c>
-      <c r="F46" s="143" t="s">
-        <v>137</v>
       </c>
       <c r="G46" s="82"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="84" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D47" s="84" t="s">
+        <v>137</v>
+      </c>
+      <c r="E47" s="84" t="s">
         <v>138</v>
       </c>
-      <c r="E47" s="84" t="s">
+      <c r="F47" s="143" t="s">
         <v>139</v>
-      </c>
-      <c r="F47" s="143" t="s">
-        <v>140</v>
       </c>
       <c r="G47" s="82"/>
       <c r="H47" s="72"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="84" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D48" s="84" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="84" t="s">
         <v>141</v>
       </c>
-      <c r="E48" s="84" t="s">
+      <c r="F48" s="143" t="s">
         <v>142</v>
-      </c>
-      <c r="F48" s="143" t="s">
-        <v>143</v>
       </c>
       <c r="G48" s="82"/>
       <c r="H48" s="72"/>
@@ -5471,7 +5594,7 @@
       </c>
       <c r="C5" s="158"/>
       <c r="D5" s="159" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="159"/>
       <c r="F5" s="159"/>
@@ -5520,7 +5643,7 @@
         <v>31</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H11" s="77" t="s">
         <v>23</v>
@@ -5723,7 +5846,7 @@
       <c r="A32" s="151"/>
       <c r="B32" s="151"/>
       <c r="C32" s="140" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D32" s="69"/>
       <c r="E32" s="69"/>
@@ -5734,19 +5857,19 @@
     </row>
     <row r="33" spans="3:8" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="141" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="141" t="s">
         <v>150</v>
       </c>
-      <c r="D33" s="141" t="s">
+      <c r="E33" s="141" t="s">
         <v>151</v>
       </c>
-      <c r="E33" s="141" t="s">
+      <c r="F33" s="141" t="s">
         <v>152</v>
       </c>
-      <c r="F33" s="141" t="s">
-        <v>153</v>
-      </c>
       <c r="G33" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H33" s="77" t="s">
         <v>23</v>
@@ -5754,64 +5877,64 @@
     </row>
     <row r="34" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C34" s="71" t="s">
+        <v>184</v>
+      </c>
+      <c r="D34" s="71" t="s">
         <v>185</v>
       </c>
-      <c r="D34" s="71" t="s">
+      <c r="E34" s="71" t="s">
         <v>186</v>
       </c>
-      <c r="E34" s="71" t="s">
+      <c r="F34" s="71" t="s">
         <v>187</v>
-      </c>
-      <c r="F34" s="71" t="s">
-        <v>188</v>
       </c>
       <c r="G34" s="82"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C35" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="71" t="s">
         <v>158</v>
       </c>
-      <c r="D35" s="71" t="s">
+      <c r="E35" s="71" t="s">
+        <v>188</v>
+      </c>
+      <c r="F35" s="71" t="s">
         <v>159</v>
-      </c>
-      <c r="E35" s="71" t="s">
-        <v>189</v>
-      </c>
-      <c r="F35" s="71" t="s">
-        <v>160</v>
       </c>
       <c r="G35" s="82"/>
       <c r="H35" s="72"/>
     </row>
     <row r="36" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C36" s="71" t="s">
+        <v>189</v>
+      </c>
+      <c r="D36" s="71" t="s">
         <v>190</v>
       </c>
-      <c r="D36" s="71" t="s">
+      <c r="E36" s="71" t="s">
+        <v>188</v>
+      </c>
+      <c r="F36" s="71" t="s">
         <v>191</v>
-      </c>
-      <c r="E36" s="71" t="s">
-        <v>189</v>
-      </c>
-      <c r="F36" s="71" t="s">
-        <v>192</v>
       </c>
       <c r="G36" s="82"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C37" s="71" t="s">
+        <v>192</v>
+      </c>
+      <c r="D37" s="71" t="s">
         <v>193</v>
-      </c>
-      <c r="D37" s="71" t="s">
-        <v>194</v>
       </c>
       <c r="E37" s="71">
         <v>800</v>
       </c>
       <c r="F37" s="71" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G37" s="82"/>
       <c r="H37" s="72"/>
@@ -5819,7 +5942,7 @@
     <row r="38" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C38" s="71"/>
       <c r="D38" s="71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E38" s="71"/>
       <c r="F38" s="71"/>
@@ -5828,48 +5951,48 @@
     </row>
     <row r="39" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C39" s="71" t="s">
+        <v>196</v>
+      </c>
+      <c r="D39" s="71" t="s">
         <v>197</v>
       </c>
-      <c r="D39" s="71" t="s">
+      <c r="E39" s="71" t="s">
         <v>198</v>
       </c>
-      <c r="E39" s="71" t="s">
+      <c r="F39" s="71" t="s">
         <v>199</v>
-      </c>
-      <c r="F39" s="71" t="s">
-        <v>200</v>
       </c>
       <c r="G39" s="82"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C40" s="71" t="s">
+        <v>200</v>
+      </c>
+      <c r="D40" s="71" t="s">
         <v>201</v>
       </c>
-      <c r="D40" s="71" t="s">
+      <c r="E40" s="71" t="s">
         <v>202</v>
       </c>
-      <c r="E40" s="71" t="s">
+      <c r="F40" s="71" t="s">
         <v>203</v>
-      </c>
-      <c r="F40" s="71" t="s">
-        <v>204</v>
       </c>
       <c r="G40" s="82"/>
       <c r="H40" s="72"/>
     </row>
     <row r="41" spans="3:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C41" s="71" t="s">
+        <v>204</v>
+      </c>
+      <c r="D41" s="71" t="s">
         <v>205</v>
       </c>
-      <c r="D41" s="71" t="s">
+      <c r="E41" s="71" t="s">
         <v>206</v>
       </c>
-      <c r="E41" s="71" t="s">
+      <c r="F41" s="71" t="s">
         <v>207</v>
-      </c>
-      <c r="F41" s="71" t="s">
-        <v>208</v>
       </c>
       <c r="G41" s="82"/>
       <c r="H41" s="72"/>
@@ -5936,7 +6059,7 @@
       </c>
       <c r="C5" s="158"/>
       <c r="D5" s="159" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="159"/>
       <c r="F5" s="159"/>
@@ -5985,7 +6108,7 @@
         <v>31</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H11" s="77" t="s">
         <v>23</v>
@@ -6188,7 +6311,7 @@
       <c r="A32" s="151"/>
       <c r="B32" s="151"/>
       <c r="C32" s="140" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D32" s="69"/>
       <c r="E32" s="69"/>
@@ -6199,19 +6322,19 @@
     </row>
     <row r="33" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="141" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="141" t="s">
         <v>150</v>
       </c>
-      <c r="D33" s="141" t="s">
+      <c r="E33" s="141" t="s">
         <v>151</v>
       </c>
-      <c r="E33" s="141" t="s">
+      <c r="F33" s="141" t="s">
         <v>152</v>
       </c>
-      <c r="F33" s="141" t="s">
-        <v>153</v>
-      </c>
       <c r="G33" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H33" s="77" t="s">
         <v>23</v>
@@ -6219,64 +6342,64 @@
     </row>
     <row r="34" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C34" s="71" t="s">
+        <v>184</v>
+      </c>
+      <c r="D34" s="71" t="s">
         <v>185</v>
       </c>
-      <c r="D34" s="71" t="s">
-        <v>186</v>
-      </c>
       <c r="E34" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="F34" s="71" t="s">
         <v>209</v>
-      </c>
-      <c r="F34" s="71" t="s">
-        <v>210</v>
       </c>
       <c r="G34" s="82"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C35" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="71" t="s">
         <v>158</v>
       </c>
-      <c r="D35" s="71" t="s">
+      <c r="E35" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="F35" s="71" t="s">
         <v>159</v>
-      </c>
-      <c r="E35" s="71" t="s">
-        <v>209</v>
-      </c>
-      <c r="F35" s="71" t="s">
-        <v>160</v>
       </c>
       <c r="G35" s="82"/>
       <c r="H35" s="72"/>
     </row>
     <row r="36" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C36" s="71" t="s">
+        <v>164</v>
+      </c>
+      <c r="D36" s="71" t="s">
         <v>165</v>
       </c>
-      <c r="D36" s="71" t="s">
-        <v>166</v>
-      </c>
       <c r="E36" s="71" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F36" s="71" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G36" s="82"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C37" s="71" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" s="71" t="s">
         <v>169</v>
-      </c>
-      <c r="D37" s="71" t="s">
-        <v>170</v>
       </c>
       <c r="E37" s="71">
         <v>2</v>
       </c>
       <c r="F37" s="71" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G37" s="82"/>
       <c r="H37" s="72"/>
@@ -6286,7 +6409,7 @@
       <c r="A39" s="151"/>
       <c r="B39" s="151"/>
       <c r="C39" s="140" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D39" s="69"/>
       <c r="E39" s="69"/>
@@ -6297,19 +6420,19 @@
     </row>
     <row r="40" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="141" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D40" s="141" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="141" t="s">
+        <v>150</v>
+      </c>
+      <c r="F40" s="141" t="s">
         <v>173</v>
       </c>
-      <c r="E40" s="141" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" s="141" t="s">
-        <v>174</v>
-      </c>
       <c r="G40" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H40" s="77" t="s">
         <v>23</v>
@@ -6317,208 +6440,208 @@
     </row>
     <row r="41" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="D41" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="E41" s="71" t="s">
         <v>213</v>
       </c>
-      <c r="D41" s="71" t="s">
-        <v>213</v>
-      </c>
-      <c r="E41" s="71" t="s">
+      <c r="F41" s="142" t="s">
         <v>214</v>
-      </c>
-      <c r="F41" s="142" t="s">
-        <v>215</v>
       </c>
       <c r="G41" s="82"/>
       <c r="H41" s="72"/>
     </row>
     <row r="42" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="71" t="s">
+        <v>215</v>
+      </c>
+      <c r="D42" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="E42" s="71" t="s">
+        <v>213</v>
+      </c>
+      <c r="F42" s="143" t="s">
         <v>216</v>
-      </c>
-      <c r="D42" s="71" t="s">
-        <v>213</v>
-      </c>
-      <c r="E42" s="71" t="s">
-        <v>214</v>
-      </c>
-      <c r="F42" s="143" t="s">
-        <v>217</v>
       </c>
       <c r="G42" s="82"/>
       <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="D43" s="71" t="s">
         <v>218</v>
       </c>
-      <c r="D43" s="71" t="s">
+      <c r="E43" s="71" t="s">
         <v>219</v>
       </c>
-      <c r="E43" s="71" t="s">
+      <c r="F43" s="143" t="s">
         <v>220</v>
-      </c>
-      <c r="F43" s="143" t="s">
-        <v>221</v>
       </c>
       <c r="G43" s="82"/>
       <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="D44" s="71" t="s">
         <v>222</v>
       </c>
-      <c r="D44" s="71" t="s">
+      <c r="E44" s="71" t="s">
         <v>223</v>
       </c>
-      <c r="E44" s="71" t="s">
+      <c r="F44" s="143" t="s">
         <v>224</v>
-      </c>
-      <c r="F44" s="143" t="s">
-        <v>225</v>
       </c>
       <c r="G44" s="82"/>
       <c r="H44" s="72"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="D45" s="71" t="s">
         <v>226</v>
       </c>
-      <c r="D45" s="71" t="s">
+      <c r="E45" s="71" t="s">
         <v>227</v>
       </c>
-      <c r="E45" s="71" t="s">
+      <c r="F45" s="143" t="s">
         <v>228</v>
-      </c>
-      <c r="F45" s="143" t="s">
-        <v>229</v>
       </c>
       <c r="G45" s="82"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="71" t="s">
+        <v>229</v>
+      </c>
+      <c r="D46" s="71" t="s">
         <v>230</v>
       </c>
-      <c r="D46" s="71" t="s">
+      <c r="E46" s="71" t="s">
         <v>231</v>
       </c>
-      <c r="E46" s="71" t="s">
+      <c r="F46" s="143" t="s">
         <v>232</v>
-      </c>
-      <c r="F46" s="143" t="s">
-        <v>233</v>
       </c>
       <c r="G46" s="82"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="71" t="s">
+        <v>233</v>
+      </c>
+      <c r="D47" s="71" t="s">
+        <v>233</v>
+      </c>
+      <c r="E47" s="71" t="s">
         <v>234</v>
       </c>
-      <c r="D47" s="71" t="s">
-        <v>234</v>
-      </c>
-      <c r="E47" s="71" t="s">
+      <c r="F47" s="143" t="s">
         <v>235</v>
-      </c>
-      <c r="F47" s="143" t="s">
-        <v>236</v>
       </c>
       <c r="G47" s="82"/>
       <c r="H47" s="72"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="71" t="s">
+        <v>236</v>
+      </c>
+      <c r="D48" s="71" t="s">
+        <v>236</v>
+      </c>
+      <c r="E48" s="71" t="s">
         <v>237</v>
       </c>
-      <c r="D48" s="71" t="s">
-        <v>237</v>
-      </c>
-      <c r="E48" s="71" t="s">
-        <v>238</v>
-      </c>
       <c r="F48" s="143" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G48" s="82"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="3:8" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D49" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="E49" s="71" t="s">
         <v>227</v>
       </c>
-      <c r="E49" s="71" t="s">
+      <c r="F49" s="143" t="s">
         <v>228</v>
-      </c>
-      <c r="F49" s="143" t="s">
-        <v>229</v>
       </c>
       <c r="G49" s="82"/>
       <c r="H49" s="72"/>
     </row>
     <row r="50" spans="3:8" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="71" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D50" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="E50" s="71" t="s">
         <v>227</v>
       </c>
-      <c r="E50" s="71" t="s">
+      <c r="F50" s="143" t="s">
         <v>228</v>
-      </c>
-      <c r="F50" s="143" t="s">
-        <v>229</v>
       </c>
       <c r="G50" s="82"/>
       <c r="H50" s="72"/>
     </row>
     <row r="51" spans="3:8" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="71" t="s">
+        <v>239</v>
+      </c>
+      <c r="D51" s="71" t="s">
         <v>240</v>
       </c>
-      <c r="D51" s="71" t="s">
+      <c r="E51" s="71" t="s">
         <v>241</v>
       </c>
-      <c r="E51" s="71" t="s">
+      <c r="F51" s="143" t="s">
         <v>242</v>
-      </c>
-      <c r="F51" s="143" t="s">
-        <v>243</v>
       </c>
       <c r="G51" s="82"/>
       <c r="H51" s="72"/>
     </row>
     <row r="52" spans="3:8" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="71" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D52" s="71" t="s">
+        <v>240</v>
+      </c>
+      <c r="E52" s="71" t="s">
         <v>241</v>
       </c>
-      <c r="E52" s="71" t="s">
+      <c r="F52" s="143" t="s">
         <v>242</v>
-      </c>
-      <c r="F52" s="143" t="s">
-        <v>243</v>
       </c>
       <c r="G52" s="82"/>
       <c r="H52" s="72"/>
     </row>
     <row r="53" spans="3:8" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="71" t="s">
+        <v>244</v>
+      </c>
+      <c r="D53" s="71" t="s">
         <v>245</v>
       </c>
-      <c r="D53" s="71" t="s">
+      <c r="E53" s="71" t="s">
         <v>246</v>
       </c>
-      <c r="E53" s="71" t="s">
+      <c r="F53" s="117" t="s">
         <v>247</v>
-      </c>
-      <c r="F53" s="117" t="s">
-        <v>248</v>
       </c>
       <c r="G53" s="82"/>
       <c r="H53" s="72"/>
@@ -6588,7 +6711,7 @@
       </c>
       <c r="C4" s="153"/>
       <c r="D4" s="154" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E4" s="154"/>
       <c r="F4" s="154"/>
@@ -6601,7 +6724,7 @@
       </c>
       <c r="C5" s="158"/>
       <c r="D5" s="159" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E5" s="159"/>
       <c r="F5" s="159"/>
@@ -6650,7 +6773,7 @@
         <v>31</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H11" s="77" t="s">
         <v>23</v>
@@ -6661,7 +6784,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="80" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -6853,7 +6976,7 @@
       <c r="A32" s="151"/>
       <c r="B32" s="151"/>
       <c r="C32" s="140" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D32" s="69"/>
       <c r="E32" s="69"/>
@@ -6864,19 +6987,19 @@
     </row>
     <row r="33" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="141" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="141" t="s">
         <v>150</v>
       </c>
-      <c r="D33" s="141" t="s">
+      <c r="E33" s="141" t="s">
         <v>151</v>
       </c>
-      <c r="E33" s="141" t="s">
+      <c r="F33" s="141" t="s">
         <v>152</v>
       </c>
-      <c r="F33" s="141" t="s">
-        <v>153</v>
-      </c>
       <c r="G33" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H33" s="77" t="s">
         <v>23</v>
@@ -6884,16 +7007,16 @@
     </row>
     <row r="34" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C34" s="71" t="s">
+        <v>249</v>
+      </c>
+      <c r="D34" s="71" t="s">
         <v>250</v>
-      </c>
-      <c r="D34" s="71" t="s">
-        <v>251</v>
       </c>
       <c r="E34" s="71">
         <v>3</v>
       </c>
       <c r="F34" s="71" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G34" s="82"/>
       <c r="H34" s="72"/>
@@ -6903,7 +7026,7 @@
       <c r="A36" s="151"/>
       <c r="B36" s="151"/>
       <c r="C36" s="140" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D36" s="69"/>
       <c r="E36" s="69"/>
@@ -6914,19 +7037,19 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="141" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="141" t="s">
         <v>150</v>
       </c>
-      <c r="D37" s="141" t="s">
+      <c r="E37" s="141" t="s">
         <v>151</v>
       </c>
-      <c r="E37" s="141" t="s">
+      <c r="F37" s="141" t="s">
         <v>152</v>
       </c>
-      <c r="F37" s="141" t="s">
-        <v>153</v>
-      </c>
       <c r="G37" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H37" s="77" t="s">
         <v>23</v>
@@ -6934,48 +7057,48 @@
     </row>
     <row r="38" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C38" s="71" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" s="71" t="s">
         <v>185</v>
       </c>
-      <c r="D38" s="71" t="s">
-        <v>186</v>
-      </c>
       <c r="E38" s="71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F38" s="71" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G38" s="82"/>
       <c r="H38" s="72"/>
     </row>
     <row r="39" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C39" s="71" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" s="71" t="s">
         <v>169</v>
-      </c>
-      <c r="D39" s="71" t="s">
-        <v>170</v>
       </c>
       <c r="E39" s="71">
         <v>3</v>
       </c>
       <c r="F39" s="71" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G39" s="82"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C40" s="71" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" s="71" t="s">
         <v>165</v>
       </c>
-      <c r="D40" s="71" t="s">
-        <v>166</v>
-      </c>
       <c r="E40" s="71" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F40" s="71" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G40" s="82"/>
       <c r="H40" s="72"/>
@@ -6985,7 +7108,7 @@
       <c r="A42" s="151"/>
       <c r="B42" s="151"/>
       <c r="C42" s="140" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D42" s="69"/>
       <c r="E42" s="69"/>
@@ -6996,19 +7119,19 @@
     </row>
     <row r="43" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="141" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D43" s="141" t="s">
+        <v>172</v>
+      </c>
+      <c r="E43" s="141" t="s">
+        <v>150</v>
+      </c>
+      <c r="F43" s="141" t="s">
         <v>173</v>
       </c>
-      <c r="E43" s="141" t="s">
-        <v>151</v>
-      </c>
-      <c r="F43" s="141" t="s">
-        <v>174</v>
-      </c>
       <c r="G43" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H43" s="77" t="s">
         <v>23</v>
@@ -7016,96 +7139,96 @@
     </row>
     <row r="44" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="71" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" s="71" t="s">
         <v>259</v>
       </c>
-      <c r="D44" s="71" t="s">
+      <c r="E44" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="E44" s="71" t="s">
+      <c r="F44" s="142" t="s">
         <v>261</v>
-      </c>
-      <c r="F44" s="142" t="s">
-        <v>262</v>
       </c>
       <c r="G44" s="82"/>
       <c r="H44" s="72"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D45" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="E45" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="E45" s="71" t="s">
+      <c r="F45" s="143" t="s">
         <v>261</v>
-      </c>
-      <c r="F45" s="143" t="s">
-        <v>262</v>
       </c>
       <c r="G45" s="82"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="71" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D46" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="E46" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="E46" s="71" t="s">
+      <c r="F46" s="143" t="s">
         <v>261</v>
-      </c>
-      <c r="F46" s="143" t="s">
-        <v>262</v>
       </c>
       <c r="G46" s="82"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="71" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D47" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="E47" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="E47" s="71" t="s">
+      <c r="F47" s="143" t="s">
         <v>261</v>
-      </c>
-      <c r="F47" s="143" t="s">
-        <v>262</v>
       </c>
       <c r="G47" s="82"/>
       <c r="H47" s="72"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="71" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D48" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="E48" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="E48" s="71" t="s">
+      <c r="F48" s="143" t="s">
         <v>261</v>
-      </c>
-      <c r="F48" s="143" t="s">
-        <v>262</v>
       </c>
       <c r="G48" s="82"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="3:8" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="71" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D49" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="E49" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="E49" s="71" t="s">
+      <c r="F49" s="143" t="s">
         <v>261</v>
-      </c>
-      <c r="F49" s="143" t="s">
-        <v>262</v>
       </c>
       <c r="G49" s="82"/>
       <c r="H49" s="72"/>
@@ -7114,17 +7237,17 @@
     <row r="51" spans="3:8" collapsed="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A32:B32"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:H5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:H6"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F44" r:id="rId1" display="https://toniapedersen.github.io/DEXPI/Symbols/ND0006_Detail.svg" xr:uid="{D281FB83-A773-40C5-913D-4FDA50BBD672}"/>
@@ -7139,6 +7262,70 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="02f74cf1-ae9f-400d-bc52-3bcd3a9e177f" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Equinor Document" ma:contentTypeID="0x01010021A623C39873404E8BA89587BD4428B401009A8AF377237CCD489B21981377E1031B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="511995c57b510c9b9ef2d21bec3a51aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="8c9155d4-e74d-4ddf-b793-2fc1446a1e11" xmlns:ns3="5b4e24bb-367d-45dc-b637-097f3fb44482" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns5="939a4e90-8150-441d-92ec-494d88fde56a" xmlns:ns6="112f239c-1cee-47a2-84cd-4b883f0f0151" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="58c44080a27012ae2e55c646ba85855d" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7478,70 +7665,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="02f74cf1-ae9f-400d-bc52-3bcd3a9e177f" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7640,6 +7763,30 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58798BDD-B71D-430A-84C4-E538830FBE77}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0452D6-5784-4571-BBD8-6297671866A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C569CB33-BC09-41FB-AA31-DACD409B820E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5337270A-D4E5-48D9-B131-BA4BD31845B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7662,30 +7809,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C569CB33-BC09-41FB-AA31-DACD409B820E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0452D6-5784-4571-BBD8-6297671866A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58798BDD-B71D-430A-84C4-E538830FBE77}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29CC7634-3062-484F-83DB-212AC7DEF6B7}">
   <ds:schemaRefs>

</xml_diff>